<commit_message>
Changed some file names and added a file in Final folder"
</commit_message>
<xml_diff>
--- a/Testing/Electrostatic Sensor/Histograms.xlsx
+++ b/Testing/Electrostatic Sensor/Histograms.xlsx
@@ -3804,7 +3804,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>Diffrence</a:t>
+              <a:t>Difference</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-NZ" baseline="0"/>
@@ -9912,8 +9912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C63" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
+      <selection activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>